<commit_message>
updated mappings for ggz usecase
</commit_message>
<xml_diff>
--- a/Mappings/FamilySituation - STU3.xlsx
+++ b/Mappings/FamilySituation - STU3.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stijn-nadm\Documents\Mijn docs\git\nictiz-stu3-zib2017\Mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nicitz-stu3-zibs2017\Mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27498" windowHeight="13998"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995"/>
   </bookViews>
   <sheets>
     <sheet name="ZIB 2017" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="114">
   <si>
     <t>Concept</t>
   </si>
@@ -353,19 +353,16 @@
     <t>SNOMED CT: 224525003 Number in household --&gt; BITS issue inschieten</t>
   </si>
   <si>
-    <t>Observation.subject(Patient) revinclude relatedperson</t>
-  </si>
-  <si>
-    <t>RelatedPerson.birthDate</t>
-  </si>
-  <si>
-    <t>RelatedPerson.extension.LivesWithPatient</t>
-  </si>
-  <si>
-    <t>Resident</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 224085006 - Family details / household composition (observable entity) / 365470003- Finding of family details and household composition (finding)</t>
+  </si>
+  <si>
+    <t>Marital status is captured through the Patient</t>
+  </si>
+  <si>
+    <t>Observation.component.extension</t>
+  </si>
+  <si>
+    <t>Observation.component</t>
   </si>
 </sst>
 </file>
@@ -610,9 +607,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Neutraal" xfId="2" builtinId="28"/>
-    <cellStyle name="Ongeldig" xfId="1" builtinId="27"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -628,7 +625,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -703,23 +700,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -755,23 +735,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -951,26 +914,26 @@
   <dimension ref="B2:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="26.41015625" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
     <col min="9" max="10" width="5" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="75" customWidth="1"/>
-    <col min="14" max="14" width="25.41015625" customWidth="1"/>
-    <col min="15" max="15" width="12.41015625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="27.87890625" customWidth="1"/>
-    <col min="17" max="17" width="71.87890625" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="27.85546875" customWidth="1"/>
+    <col min="17" max="17" width="71.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +973,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="77.400000000000006" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:17" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +997,7 @@
         <v>13</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
@@ -1044,7 +1007,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="103.2" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:17" ht="102" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
       <c r="C4" s="13" t="s">
         <v>14</v>
@@ -1076,9 +1039,11 @@
       <c r="P4" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="Q4" s="2"/>
-    </row>
-    <row r="5" spans="2:17" ht="38.700000000000003" x14ac:dyDescent="0.5">
+      <c r="Q4" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
         <v>21</v>
@@ -1116,7 +1081,7 @@
       </c>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
       <c r="C6" s="13" t="s">
         <v>28</v>
@@ -1152,7 +1117,7 @@
       </c>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="2:17" ht="38.700000000000003" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
       <c r="C7" s="13" t="s">
         <v>34</v>
@@ -1188,7 +1153,7 @@
       </c>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
       <c r="C8" s="13" t="s">
         <v>38</v>
@@ -1224,7 +1189,7 @@
       </c>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B9" s="15"/>
       <c r="C9" s="16" t="s">
         <v>44</v>
@@ -1254,11 +1219,11 @@
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13" t="s">
@@ -1290,11 +1255,11 @@
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="20" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="Q10" s="20"/>
     </row>
-    <row r="11" spans="2:17" ht="38.700000000000003" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13" t="s">
@@ -1328,11 +1293,9 @@
       <c r="P11" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="Q11" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="Q11" s="20"/>
+    </row>
+    <row r="12" spans="2:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="C12" s="13" t="s">
         <v>61</v>
@@ -1388,7 +1351,7 @@
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -1397,7 +1360,7 @@
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C3" s="23" t="s">
         <v>27</v>
       </c>
@@ -1408,7 +1371,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" s="18" t="s">
         <v>67</v>
       </c>
@@ -1425,7 +1388,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>72</v>
       </c>
@@ -1442,7 +1405,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>77</v>
       </c>
@@ -1459,7 +1422,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>80</v>
       </c>
@@ -1476,7 +1439,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>83</v>
       </c>
@@ -1493,7 +1456,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>86</v>
       </c>
@@ -1510,7 +1473,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>89</v>
       </c>
@@ -1527,7 +1490,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
         <v>92</v>
       </c>
@@ -1544,7 +1507,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
finished FamilySituation, updated respective mapping xlsx
</commit_message>
<xml_diff>
--- a/Mappings/FamilySituation - STU3.xlsx
+++ b/Mappings/FamilySituation - STU3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="117">
   <si>
     <t>Concept</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Observation.component.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">SNOMED CT: </t>
-  </si>
-  <si>
     <t>SNOMED CT:</t>
   </si>
   <si>
@@ -353,9 +350,6 @@
     <t>SNOMED CT: 224525003 Number in household --&gt; BITS issue inschieten</t>
   </si>
   <si>
-    <t xml:space="preserve"> 224085006 - Family details / household composition (observable entity) / 365470003- Finding of family details and household composition (finding)</t>
-  </si>
-  <si>
     <t>Marital status is captured through the Patient</t>
   </si>
   <si>
@@ -363,13 +357,29 @@
   </si>
   <si>
     <t>Observation.component</t>
+  </si>
+  <si>
+    <t>55811000146107 |Number of children living at home (observable entity)|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">224130005 |Household composition (observable entity)|
+</t>
+  </si>
+  <si>
+    <t>Observation.component.valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>Observation.component.valueQuantity</t>
+  </si>
+  <si>
+    <t>365470003- Finding of family details and household composition (finding)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -418,8 +428,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,8 +472,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -528,13 +549,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -605,9 +642,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -914,7 +964,7 @@
   <dimension ref="B2:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -973,7 +1023,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
@@ -996,15 +1046,15 @@
       <c r="M3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="21" t="s">
-        <v>110</v>
+      <c r="N3" s="27" t="s">
+        <v>116</v>
       </c>
       <c r="O3" s="4"/>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="24" t="s">
         <v>102</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="2:17" ht="102" x14ac:dyDescent="0.2">
@@ -1036,14 +1086,14 @@
       <c r="O4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="24" t="s">
         <v>103</v>
       </c>
       <c r="Q4" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" ht="38.25" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="51" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
         <v>21</v>
@@ -1070,14 +1120,14 @@
       <c r="M5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="21" t="s">
-        <v>105</v>
+      <c r="N5" s="26" t="s">
+        <v>113</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="20" t="s">
-        <v>104</v>
+      <c r="P5" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="Q5" s="2"/>
     </row>
@@ -1108,12 +1158,12 @@
       <c r="M6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="20" t="s">
         <v>33</v>
       </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="20" t="s">
-        <v>104</v>
+      <c r="P6" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="Q6" s="2"/>
     </row>
@@ -1144,12 +1194,12 @@
       <c r="M7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="21" t="s">
-        <v>106</v>
+      <c r="N7" s="25" t="s">
+        <v>112</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="20" t="s">
-        <v>104</v>
+      <c r="P7" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="Q7" s="2"/>
     </row>
@@ -1181,7 +1231,7 @@
         <v>43</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="20" t="s">
@@ -1219,7 +1269,7 @@
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Q9" s="5"/>
     </row>
@@ -1287,11 +1337,11 @@
         <v>60</v>
       </c>
       <c r="N11" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q11" s="20"/>
     </row>
@@ -1326,8 +1376,8 @@
         <v>65</v>
       </c>
       <c r="O12" s="2"/>
-      <c r="P12" s="20" t="s">
-        <v>107</v>
+      <c r="P12" s="24" t="s">
+        <v>106</v>
       </c>
       <c r="Q12" s="2"/>
     </row>

</xml_diff>